<commit_message>
Filled Green color for Ega and Ram
</commit_message>
<xml_diff>
--- a/TeamDetails.xlsx
+++ b/TeamDetails.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egambarampanneerselvam/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egambarampanneerselvam/MyLearning/GitHubDemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93B78551-4C0D-3B4B-ADE6-44E48A35D846}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49895119-866E-CB48-AB02-F4022DA22F72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="460" windowWidth="24500" windowHeight="15000" xr2:uid="{67415C8B-937D-2C40-BDAE-6A09BB706631}"/>
   </bookViews>
@@ -130,12 +130,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -165,13 +171,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE08598-1662-BA48-A5DA-BD887D4DB0ED}">
-  <dimension ref="B1:D14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -514,7 +521,7 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -525,7 +532,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">

</xml_diff>